<commit_message>
Added Floor and Ceiling functions and document detailing how to add a new database function.
</commit_message>
<xml_diff>
--- a/test/HatTrick.DbEx.MsSql.Test.Database/Executor/_Functions/_Interactions/mssql_function_interaction_matrix.xlsx
+++ b/test/HatTrick.DbEx.MsSql.Test.Database/Executor/_Functions/_Interactions/mssql_function_interaction_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\db-ex\test\HatTrick.DbEx.MsSql.Test.Database\Executor\_Functions\_Interactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD10B2EE-EB70-4AFF-BFBB-05E722CBBB5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13BC22-C279-404A-8E68-6D641E29E072}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="1185" windowWidth="21915" windowHeight="16665" xr2:uid="{0B321049-17AF-4334-90B2-A285CDF0541B}"/>
+    <workbookView xWindow="2520" yWindow="2535" windowWidth="34875" windowHeight="15870" xr2:uid="{0B321049-17AF-4334-90B2-A285CDF0541B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Average</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Covered</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Ceiling</t>
   </si>
 </sst>
 </file>
@@ -114,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,11 +177,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A65D068-0606-48D0-AF9E-3811A000EC86}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -500,412 +512,486 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="R2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>